<commit_message>
modified:   app/Http/Controllers/EmployeeController.php 	modified:   app/Http/Requests/EmployeeStoreRequest.php 	modified:   app/Models/Employee.php 	modified:   database/migrations/2022_01_27_040750_update_alter_employees_table.php 	modified:   database/seeders/companies.xlsx 	modified:   database/seeders/companies/companies.md 	modified:   database/seeders/employees.xlsx 	modified:   database/seeders/employees/employees.md 	modified:   database/seeders/items.xlsx 	modified:   database/seeders/sell_summaries.xlsx 	modified:   database/seeders/sell_summaries/sell_summaries.md 	modified:   database/seeders/sells.xlsx 	modified:   database/seeders/sells/sells.md 	modified:   resources/views/employee/create.blade.php 	modified:   resources/views/employee/edit.blade.php 	modified:   tests/Feature/EmployeeTest.php
</commit_message>
<xml_diff>
--- a/database/seeders/items.xlsx
+++ b/database/seeders/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CRM\database\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17CD8773-79F7-4294-878A-734F19DCD8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CB8503-0CCB-4E2D-9E2C-12573F47BD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items (1)" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -950,12 +950,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>